<commit_message>
add 3 bank models
</commit_message>
<xml_diff>
--- a/fridaa_ocr/knowledge_base/alim_keywords.xlsx
+++ b/fridaa_ocr/knowledge_base/alim_keywords.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24606"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="141" documentId="11_7C1ED94ECBD35814F8F49F9D1D27DCCF8F4A0B19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F22BF9E-B644-4042-A3AA-450B911C7670}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="11_7C1ED94ECBD35814F8F49F9D1D27DCCF8F4A0B19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0DBA8B0-DFAB-4825-B792-BDC8B2FA58D2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>variables</t>
   </si>
@@ -40,7 +40,10 @@
     <t>LCL</t>
   </si>
   <si>
-    <t>Caisse D'epargne</t>
+    <t>Caisse d'Epargne</t>
+  </si>
+  <si>
+    <t>BNP</t>
   </si>
   <si>
     <t>Revenus Mensuels</t>
@@ -52,6 +55,9 @@
     <t>Revenus globaux annuels pour l'ensemble des emprunteurs</t>
   </si>
   <si>
+    <t>__NULL__</t>
+  </si>
+  <si>
     <t>revenus mensuels</t>
   </si>
   <si>
@@ -70,64 +76,88 @@
     <t>Crédits en cours</t>
   </si>
   <si>
+    <t>Apport personnel</t>
+  </si>
+  <si>
+    <t>Fonds propres de l'emprunteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apport personnel </t>
+  </si>
+  <si>
+    <t>Coût de l’acquisition</t>
+  </si>
+  <si>
+    <t>Acquisition d'ancien</t>
+  </si>
+  <si>
+    <t>Bien immobilier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montant de l'acquisition </t>
+  </si>
+  <si>
+    <t>Frais d’agence</t>
+  </si>
+  <si>
+    <t>Frais d'agence</t>
+  </si>
+  <si>
+    <t>Frais de courtage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montant des frais de courtage financés </t>
+  </si>
+  <si>
+    <t>Frais de banque</t>
+  </si>
+  <si>
+    <t>Frais de dossier</t>
+  </si>
+  <si>
+    <t>Frais de garanites</t>
+  </si>
+  <si>
+    <t>Coût des garanties</t>
+  </si>
+  <si>
+    <t>Frais de prise de garantie (SACCEF)</t>
+  </si>
+  <si>
+    <t>Frais de garantie</t>
+  </si>
+  <si>
+    <t>Estimation de la garantie</t>
+  </si>
+  <si>
+    <t>Montant emprunté</t>
+  </si>
+  <si>
+    <t>Total de nos prêts</t>
+  </si>
+  <si>
+    <t>Montant total des prêts de la banque</t>
+  </si>
+  <si>
+    <t>Solution Projet Immo a taux fixe</t>
+  </si>
+  <si>
+    <t>Prêts Caisse d'Epargne</t>
+  </si>
+  <si>
+    <t>Habitat TF</t>
+  </si>
+  <si>
+    <t>Montant total des intérêts</t>
+  </si>
+  <si>
     <t>NR</t>
   </si>
   <si>
-    <t>Apport personnel</t>
-  </si>
-  <si>
-    <t>Fonds propres de l'emprunteur</t>
-  </si>
-  <si>
-    <t>Apport personnel :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apport personnel </t>
-  </si>
-  <si>
-    <t>Coût de l’acquisition</t>
-  </si>
-  <si>
-    <t>Acquisition d'ancien</t>
-  </si>
-  <si>
-    <t>Bien immobilier</t>
-  </si>
-  <si>
-    <t>Frais d’agence</t>
-  </si>
-  <si>
-    <t>Frais d'agence</t>
-  </si>
-  <si>
-    <t>Frais de courtage</t>
-  </si>
-  <si>
-    <t>Frais de banque</t>
-  </si>
-  <si>
-    <t>Frais de dossier</t>
-  </si>
-  <si>
-    <t>Frais de garanites</t>
-  </si>
-  <si>
-    <t>Coût des garanties</t>
-  </si>
-  <si>
-    <t>Frais de garantie</t>
-  </si>
-  <si>
-    <t>Montant emprunté</t>
-  </si>
-  <si>
-    <t>Total de nos prêts</t>
-  </si>
-  <si>
-    <t>Prêts Caisse d'Epargne</t>
-  </si>
-  <si>
-    <t>Montant total des intérêts</t>
+    <t>Intéréts du (des) prét(s)</t>
+  </si>
+  <si>
+    <t>lntéréts</t>
   </si>
   <si>
     <t>Taux</t>
@@ -136,6 +166,9 @@
     <t>Taux Annuel Effectif Global (TAEG)</t>
   </si>
   <si>
+    <t>Taux Annuel Effectif Global "T.A.E.G."</t>
+  </si>
+  <si>
     <t>Taux Annuel Effectif Global - TAEG</t>
   </si>
   <si>
@@ -155,6 +188,9 @@
   </si>
   <si>
     <t>Frais de Notaire</t>
+  </si>
+  <si>
+    <t>Montant des frais de notaire financés</t>
   </si>
   <si>
     <t>Code postal</t>
@@ -1483,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE1BFC8-B59D-43B6-A017-F5A4B1EF7249}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1496,14 +1532,15 @@
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="11" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="11" width="12.5703125" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" customWidth="1"/>
     <col min="13" max="14" width="12.5703125" customWidth="1"/>
     <col min="15" max="16" width="14.42578125" customWidth="1"/>
     <col min="17" max="19" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1519,64 +1556,91 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="38.25">
+    <row r="2" spans="1:6" ht="38.25">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="78" customHeight="1">
+    <row r="3" spans="1:6" ht="78" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:6" ht="30">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
       </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1586,131 +1650,233 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:6" ht="38.25">
       <c r="A8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>14</v>
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45">
+    <row r="13" spans="1:6" ht="45">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>35</v>
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="45">
+    <row r="15" spans="1:6" ht="45">
       <c r="A15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>14</v>
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="45">
+    <row r="16" spans="1:6" ht="45">
       <c r="A16" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="4" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:6" ht="15">
       <c r="A18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>14</v>
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1719,6 +1885,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A53E21AADB3F9249BECE9198D0A86B6B" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="bc71084de06be6f6a0de9144acbad507">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8e174d0e-a89b-4ea6-98ae-dd46b746d8a4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b4ed9f6660d725bb720c6f62b104b8fa" ns2:_="">
     <xsd:import namespace="8e174d0e-a89b-4ea6-98ae-dd46b746d8a4"/>
@@ -1876,23 +2057,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD22EFB0-0170-4CB0-B912-BD0F26E807A4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0826C47E-8A54-4E4F-85B7-3681B339134E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1900,5 +2066,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0826C47E-8A54-4E4F-85B7-3681B339134E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD22EFB0-0170-4CB0-B912-BD0F26E807A4}"/>
 </file>
</xml_diff>